<commit_message>
rename backend to en-us
</commit_message>
<xml_diff>
--- a/setup/undermerch-template.xlsx
+++ b/setup/undermerch-template.xlsx
@@ -7,10 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Usuarios" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Produtos" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Movimentacoes" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Vendas" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Users" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Products" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Movements" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sales" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,26 +28,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E8EAF6"/>
-        <bgColor rgb="00E8EAF6"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -55,20 +45,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin">
-        <color rgb="009E9E9E"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -437,29 +419,23 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>role</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>createdAt</t>
         </is>
@@ -479,65 +455,53 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
-    <col width="13" customWidth="1" min="9" max="9"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>nome</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>descricao</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>preco</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>estoque</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>imagemId</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ativo</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>stock</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>imageId</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>createdAt</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>updatedAt</t>
         </is>
@@ -557,53 +521,43 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="16" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>produtoId</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>tipo</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>quantidade</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>motivo</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>usuarioEmail</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>productId</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>reason</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>userEmail</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
         <is>
           <t>createdAt</t>
         </is>
@@ -623,59 +577,48 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="17" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="19" customWidth="1" min="6" max="6"/>
-    <col width="16" customWidth="1" min="7" max="7"/>
-    <col width="13" customWidth="1" min="8" max="8"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>produtoId</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>quantidade</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>precoUnitario</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>productId</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>unitPrice</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
         <is>
           <t>total</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>metodoPagamento</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>usuarioEmail</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>paymentMethod</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>userEmail</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
         <is>
           <t>createdAt</t>
         </is>

</xml_diff>

<commit_message>
Add lastAccess column to Users table
Track when each user last accessed the system. The lastAccess
timestamp is updated on every login in checkAuth. The frontend
users list is now sorted by most recent access and displays the
last access date. Updated the setup template, tutorial, and plan
to reflect the new column.

https://claude.ai/code/session_01AjM5J4EQcrvycnFVfGL7mH
</commit_message>
<xml_diff>
--- a/setup/undermerch-template.xlsx
+++ b/setup/undermerch-template.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,11 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>createdAt</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>lastAccess</t>
         </is>
       </c>
     </row>
@@ -514,7 +519,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>

</xml_diff>